<commit_message>
added comments to sv juptyer notebook
</commit_message>
<xml_diff>
--- a/machine_learning/ml_summary_data.xlsx
+++ b/machine_learning/ml_summary_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike Occhicone\Desktop\DACert\fitness\fitness_tracking\machine_learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78FF00C-8498-4CCA-8622-7CC81213D1CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05546B83-1DA4-4F21-B560-35BBAA473B2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="27150" windowHeight="16440" xr2:uid="{83D5FDE1-BDB6-42AD-8D89-86B51BF8D8F3}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
   <si>
     <t>recall</t>
   </si>
@@ -79,6 +79,27 @@
   </si>
   <si>
     <t>Andrew2_no_Elliptical</t>
+  </si>
+  <si>
+    <t>Mary Robert</t>
+  </si>
+  <si>
+    <t>Linear Regression</t>
+  </si>
+  <si>
+    <t>Lasso</t>
+  </si>
+  <si>
+    <t>Ridge</t>
+  </si>
+  <si>
+    <t>ElasticNet</t>
+  </si>
+  <si>
+    <t>test_MSE</t>
+  </si>
+  <si>
+    <t>train_MSE</t>
   </si>
 </sst>
 </file>
@@ -439,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E076DF-7572-4D41-A148-9621B70B8766}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,7 +473,7 @@
     <col min="3" max="3" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -655,37 +676,113 @@
       <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="A15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="D16" s="4">
+        <v>0.98</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="E17" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="F17" s="4">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="E18" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="F18" s="4">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="E19" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="F19" s="4">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>